<commit_message>
add periode bulan using list and fix bug export
</commit_message>
<xml_diff>
--- a/directory/templates/template-absensi-custom.xlsx
+++ b/directory/templates/template-absensi-custom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\hrmis-master\directory\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4652E3-DAF4-4D5A-9C10-AC3986F2135F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6A4D82-B515-4DC1-9616-B53F5A3EDD20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{31A0B364-D528-4097-98D0-DBAC8A79801F}"/>
   </bookViews>
@@ -120,7 +120,7 @@
     <t>[jadwal_nama]</t>
   </si>
   <si>
-    <t>HRMIS | Absen</t>
+    <t>HRMIS | Absen {tanggal_periode}</t>
   </si>
 </sst>
 </file>
@@ -756,7 +756,7 @@
   <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>